<commit_message>
Add some other test case and implemented with excel file
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,17 +4,257 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
+    <sheet name="AddUserModelerUI01Test" sheetId="2" r:id="rId2"/>
+    <sheet name="AddGroupsModelerUI01Test" sheetId="3" r:id="rId3"/>
+    <sheet name="EditUserModelerUITest" sheetId="4" r:id="rId4"/>
+    <sheet name="AssignUserToGroupModelerUI" sheetId="5" r:id="rId5"/>
+    <sheet name="AddTagsToGroupTest" sheetId="6" r:id="rId6"/>
+    <sheet name="AddProjectTest" sheetId="7" r:id="rId7"/>
+    <sheet name="AddTagTest" sheetId="8" r:id="rId8"/>
+    <sheet name="AddProjectTagAndDiagram" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Just change the label value from this cell, it will change the permission accordingly</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Project Administration xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Folder Management xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Banch Manager xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision Modeler xpath</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Just change the name of the user to 'xyz' from the 'Test Undelete' place</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Just change the name of the group to 'xyz' from the 'Test Group' place</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These three are the xpath of branching, just copy and paste the xapth with the required branching in the first row and second column.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>Webelement</t>
   </si>
@@ -44,13 +284,199 @@
   </si>
   <si>
     <t>//td[@class='fieldData']//label[4]</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>Standard 6</t>
+  </si>
+  <si>
+    <t>test6@rxw.com</t>
+  </si>
+  <si>
+    <t>STANDARD</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>READER</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>DISABLED</t>
+  </si>
+  <si>
+    <t>groupName</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>permissions</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>test group</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Test Undelete')]</t>
+  </si>
+  <si>
+    <t>editUserXpath</t>
+  </si>
+  <si>
+    <t>types</t>
+  </si>
+  <si>
+    <t>Update name</t>
+  </si>
+  <si>
+    <t>//div[normalize-space()='Test Group']</t>
+  </si>
+  <si>
+    <t>groups</t>
+  </si>
+  <si>
+    <t>editGroupXpath</t>
+  </si>
+  <si>
+    <t>//div[contains(text(),'Test Group')]</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>//nb-option[contains(text(),'Add Tag Group ')]</t>
+  </si>
+  <si>
+    <t>//nb-option[contains(text(),'main')]</t>
+  </si>
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>branching</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>//nb-radio[@id='item-enableSimpleBranching']//span[@class='inner-circle']</t>
+  </si>
+  <si>
+    <t>Test dummy 9</t>
+  </si>
+  <si>
+    <t>//nb-radio[@id='item-enableBranching']//span[@class='inner-circle']</t>
+  </si>
+  <si>
+    <t>//nb-radio[@id='item-disableBranching']//span[@class='inner-circle']</t>
+  </si>
+  <si>
+    <t>searchProject</t>
+  </si>
+  <si>
+    <t>tagName</t>
+  </si>
+  <si>
+    <t>tagDescription</t>
+  </si>
+  <si>
+    <t>Test Tag</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>Twelve October</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test dummy 9 (main)']</t>
+  </si>
+  <si>
+    <t>Test Demo</t>
+  </si>
+  <si>
+    <t>projectName1</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test Demo (main)']</t>
+  </si>
+  <si>
+    <t>tagXpath</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test Tag']</t>
+  </si>
+  <si>
+    <t>diagramName</t>
+  </si>
+  <si>
+    <t>diagramDescription</t>
+  </si>
+  <si>
+    <t>Test Diagram14</t>
+  </si>
+  <si>
+    <t>description demo</t>
+  </si>
+  <si>
+    <t>inputName</t>
+  </si>
+  <si>
+    <t>decisionName</t>
+  </si>
+  <si>
+    <t>knowledgeName</t>
+  </si>
+  <si>
+    <t>Knowledge name Updated</t>
+  </si>
+  <si>
+    <t>Input name Updated</t>
+  </si>
+  <si>
+    <t>Decision name Updated</t>
+  </si>
+  <si>
+    <t>knowledgeCoordinates</t>
+  </si>
+  <si>
+    <t>InputCoordinates</t>
+  </si>
+  <si>
+    <t>DecisionCoordinates</t>
+  </si>
+  <si>
+    <t>connection links</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,13 +485,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <color rgb="FF202124"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,6 +530,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -88,15 +567,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -398,60 +894,664 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" t="s">
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
+      <c r="C7">
+        <v>-56</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>-30</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>70</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+      <c r="F8">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>155</v>
+      </c>
+      <c r="B11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>255</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>180</v>
+      </c>
+      <c r="B13">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-100</v>
+      </c>
+      <c r="B14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>180</v>
+      </c>
+      <c r="B15">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-250</v>
+      </c>
+      <c r="B16">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
adding diagram with objets and links
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="AddProjectTest" sheetId="7" r:id="rId7"/>
     <sheet name="AddTagTest" sheetId="8" r:id="rId8"/>
     <sheet name="AddProjectTagAndDiagram" sheetId="9" r:id="rId9"/>
+    <sheet name="AddDiagramWithObjectsAndLinks" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -253,8 +254,153 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Input data canvas coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Author:
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision data canvas coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of knowledge coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of goup coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of annotation coordinates</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
   <si>
     <t>Webelement</t>
   </si>
@@ -470,13 +616,40 @@
   </si>
   <si>
     <t>connection links</t>
+  </si>
+  <si>
+    <t>inputObjectCoordiates</t>
+  </si>
+  <si>
+    <t>decisionObjectCoordiates</t>
+  </si>
+  <si>
+    <t>knowledgeObjectCoordiates</t>
+  </si>
+  <si>
+    <t>groupObjectCoordiates</t>
+  </si>
+  <si>
+    <t>annnotationObjectCoordiates</t>
+  </si>
+  <si>
+    <t>informationLinkCoordinates</t>
+  </si>
+  <si>
+    <t>authorityLinkCoordinates</t>
+  </si>
+  <si>
+    <t>annotationLinkCoordinates</t>
+  </si>
+  <si>
+    <t>canvasCoordinates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,8 +692,16 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -557,6 +738,54 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -571,7 +800,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -588,6 +817,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -968,6 +1221,306 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-30</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>-56</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>58</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="D10" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="G10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-43</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-100</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>250</v>
+      </c>
+      <c r="B16">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-130</v>
+      </c>
+      <c r="B18">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>300</v>
+      </c>
+      <c r="B20">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>300</v>
+      </c>
+      <c r="B22">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
@@ -1099,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -1328,7 +1881,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adding delete customer, user , groups and executed in Openshift Env
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,11 @@
     <sheet name="AddProjectTest" sheetId="7" r:id="rId7"/>
     <sheet name="AddTagTest" sheetId="8" r:id="rId8"/>
     <sheet name="AddProjectTagAndDiagram" sheetId="9" r:id="rId9"/>
-    <sheet name="AddDiagramWithObjectsAndLinks" sheetId="10" r:id="rId10"/>
+    <sheet name="AddCustomer" sheetId="11" r:id="rId10"/>
+    <sheet name="AddDiagramWithObjectsAndLinks" sheetId="10" r:id="rId11"/>
+    <sheet name="DeleteUserModelerUI" sheetId="12" r:id="rId12"/>
+    <sheet name="DeleteGroupsModelerUI" sheetId="13" r:id="rId13"/>
+    <sheet name="DeleteCustomer" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -399,8 +403,114 @@
 </comments>
 </file>
 
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Project Administration xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Folder Management xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Banch Manager xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision Modeler xpath</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="105">
   <si>
     <t>Webelement</t>
   </si>
@@ -531,9 +641,6 @@
     <t>//nb-radio[@id='item-enableSimpleBranching']//span[@class='inner-circle']</t>
   </si>
   <si>
-    <t>Test dummy 9</t>
-  </si>
-  <si>
     <t>//nb-radio[@id='item-enableBranching']//span[@class='inner-circle']</t>
   </si>
   <si>
@@ -643,6 +750,81 @@
   </si>
   <si>
     <t>canvasCoordinates</t>
+  </si>
+  <si>
+    <t>customerName</t>
+  </si>
+  <si>
+    <t>numberOfUsers</t>
+  </si>
+  <si>
+    <t>domains</t>
+  </si>
+  <si>
+    <t>Test dummy</t>
+  </si>
+  <si>
+    <t>dummy.com</t>
+  </si>
+  <si>
+    <t>User 1</t>
+  </si>
+  <si>
+    <t>User 2</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Admin@dummy.com</t>
+  </si>
+  <si>
+    <t>//option[. = 'ADMIN']</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Standard@dummy.com</t>
+  </si>
+  <si>
+    <t>//option[. = 'STANDARD']</t>
+  </si>
+  <si>
+    <t>Test Delete User</t>
+  </si>
+  <si>
+    <t>Standard Delete</t>
+  </si>
+  <si>
+    <t>deleteuser@dummy.com</t>
+  </si>
+  <si>
+    <t>//div[normalize-space()='Test Delete User']</t>
+  </si>
+  <si>
+    <t>deleteUser</t>
+  </si>
+  <si>
+    <t>Test Delete Group</t>
+  </si>
+  <si>
+    <t>test for delete group</t>
+  </si>
+  <si>
+    <t>deleteGroup</t>
+  </si>
+  <si>
+    <t>//div[normalize-space()='Test Delete Group']</t>
+  </si>
+  <si>
+    <t>Test Delete Account</t>
+  </si>
+  <si>
+    <t>delete.com</t>
   </si>
 </sst>
 </file>
@@ -819,6 +1001,18 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -829,18 +1023,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1151,7 +1333,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1222,10 +1404,90 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -1256,39 +1518,39 @@
         <v>40</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -1297,67 +1559,67 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
       <c r="K2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
         <v>65</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>66</v>
-      </c>
-      <c r="M2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="15"/>
+      <c r="E7" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="17"/>
+      <c r="I7" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1392,16 +1654,16 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="D10" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="D10" s="15" t="s">
+      <c r="E10" s="12"/>
+      <c r="G10" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="E10" s="15"/>
-      <c r="G10" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -1426,10 +1688,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B13" s="17"/>
+      <c r="A13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1505,6 +1767,7 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I7:J7"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="G10:H10"/>
@@ -1513,11 +1776,191 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1526,7 +1969,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +2037,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,7 +2177,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,7 +2222,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,7 +2245,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -1813,12 +2256,12 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1845,30 +2288,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="B2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1881,7 +2324,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1909,39 +2352,39 @@
         <v>40</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -1950,57 +2393,57 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
       <c r="K2" t="s">
+        <v>64</v>
+      </c>
+      <c r="L2" t="s">
         <v>65</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>66</v>
-      </c>
-      <c r="M2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="8"/>
     </row>
@@ -2046,7 +2489,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="9"/>
     </row>

</xml_diff>

<commit_message>
added re-use objects and reports
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,11 @@
     <sheet name="AddTagTest" sheetId="8" r:id="rId8"/>
     <sheet name="AddProjectTagAndDiagram" sheetId="9" r:id="rId9"/>
     <sheet name="AddCustomer" sheetId="11" r:id="rId10"/>
-    <sheet name="AddDiagramWithObjectsAndLinks" sheetId="10" r:id="rId11"/>
-    <sheet name="DeleteUserModelerUI" sheetId="12" r:id="rId12"/>
-    <sheet name="DeleteGroupsModelerUI" sheetId="13" r:id="rId13"/>
-    <sheet name="DeleteCustomer" sheetId="14" r:id="rId14"/>
+    <sheet name="ReuseDiagramAndObjects" sheetId="15" r:id="rId11"/>
+    <sheet name="AddDiagramWithObjectsAndLinks" sheetId="10" r:id="rId12"/>
+    <sheet name="DeleteUserModelerUI" sheetId="12" r:id="rId13"/>
+    <sheet name="DeleteGroupsModelerUI" sheetId="13" r:id="rId14"/>
+    <sheet name="DeleteCustomer" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -409,7 +410,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="B14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -429,11 +430,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Project Administration xpath</t>
+Input data canvas coordinates</t>
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="A16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -443,21 +444,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Folder Management xpath</t>
+          <t xml:space="preserve">Author:
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -477,11 +469,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Banch Manager xpath</t>
+Decision data canvas coordinates</t>
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -501,7 +493,55 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Decision Modeler xpath</t>
+canvas value of knowledge coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of goup coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of annotation coordinates</t>
         </r>
       </text>
     </comment>
@@ -515,6 +555,112 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Project Administration xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Folder Management xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Banch Manager xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision Modeler xpath</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
     <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -544,7 +690,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="121">
   <si>
     <t>Webelement</t>
   </si>
@@ -702,15 +848,9 @@
     <t>//span[normalize-space()='Test dummy 9 (main)']</t>
   </si>
   <si>
-    <t>Test Demo</t>
-  </si>
-  <si>
     <t>projectName1</t>
   </si>
   <si>
-    <t>//span[normalize-space()='Test Demo (main)']</t>
-  </si>
-  <si>
     <t>tagXpath</t>
   </si>
   <si>
@@ -723,9 +863,6 @@
     <t>diagramDescription</t>
   </si>
   <si>
-    <t>Test Diagram14</t>
-  </si>
-  <si>
     <t>description demo</t>
   </si>
   <si>
@@ -798,9 +935,6 @@
     <t>Test dummy</t>
   </si>
   <si>
-    <t>dummy.com</t>
-  </si>
-  <si>
     <t>User 1</t>
   </si>
   <si>
@@ -813,18 +947,12 @@
     <t>Tester</t>
   </si>
   <si>
-    <t>Admin@dummy.com</t>
-  </si>
-  <si>
     <t>//option[. = 'ADMIN']</t>
   </si>
   <si>
     <t>Standard</t>
   </si>
   <si>
-    <t>Standard@dummy.com</t>
-  </si>
-  <si>
     <t>//option[. = 'STANDARD']</t>
   </si>
   <si>
@@ -865,6 +993,66 @@
   </si>
   <si>
     <t>//span[contains(text(),'Test Delete Account')]</t>
+  </si>
+  <si>
+    <t>inputData1</t>
+  </si>
+  <si>
+    <t>inputData2</t>
+  </si>
+  <si>
+    <t>decisionData1</t>
+  </si>
+  <si>
+    <t>decisionData2</t>
+  </si>
+  <si>
+    <t>decisionData3</t>
+  </si>
+  <si>
+    <t>knowledgeData1</t>
+  </si>
+  <si>
+    <t>Input Data-Nitesh (2)</t>
+  </si>
+  <si>
+    <t>Decision-Nitesh (2)</t>
+  </si>
+  <si>
+    <t>Decision-Nitesh (3)</t>
+  </si>
+  <si>
+    <t>Test Random</t>
+  </si>
+  <si>
+    <t>random.com</t>
+  </si>
+  <si>
+    <t>Admin@random.com</t>
+  </si>
+  <si>
+    <t>Standard@random.com</t>
+  </si>
+  <si>
+    <t>Test Automation</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test Automation (main)']</t>
+  </si>
+  <si>
+    <t>Test Create Diagram</t>
+  </si>
+  <si>
+    <t>Test Diagram Demo</t>
+  </si>
+  <si>
+    <t>Input Data-Nitesh (3)</t>
+  </si>
+  <si>
+    <t>Decision-Nitesh (4)</t>
+  </si>
+  <si>
+    <t>Knowledge Source-Nitesh (2)</t>
   </si>
 </sst>
 </file>
@@ -1054,15 +1242,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1076,6 +1255,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1461,7 +1649,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,73 +1663,397 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" t="s">
-        <v>92</v>
+      <c r="E4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="68.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>107</v>
+      </c>
+      <c r="L2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" t="s">
+        <v>108</v>
+      </c>
+      <c r="N2" t="s">
+        <v>109</v>
+      </c>
+      <c r="O2" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="J7" s="15"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-30</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>-56</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>58</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="D10" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="17"/>
+      <c r="G10" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>-43</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-100</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>250</v>
+      </c>
+      <c r="B16">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>-130</v>
+      </c>
+      <c r="B18">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>50</v>
+      </c>
+      <c r="B19">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>300</v>
+      </c>
+      <c r="B20">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>300</v>
+      </c>
+      <c r="B22">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,7 +2086,7 @@
         <v>45</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>46</v>
@@ -1583,27 +2095,27 @@
         <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -1612,10 +2124,10 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -1624,22 +2136,22 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1653,26 +2165,26 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
+      <c r="H7" s="14"/>
+      <c r="I7" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1707,16 +2219,16 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="D10" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="12"/>
+      <c r="A10" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="D10" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="17"/>
       <c r="G10" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -1741,10 +2253,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="13"/>
+      <c r="A13" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="10"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1836,7 +2348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1867,24 +2379,24 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,11 +2422,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
@@ -1937,21 +2449,21 @@
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1975,7 +2487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1993,30 +2505,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2306,7 +2818,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -2384,8 +2896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2416,7 +2928,7 @@
         <v>45</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>46</v>
@@ -2425,27 +2937,27 @@
         <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -2454,10 +2966,10 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -2466,22 +2978,22 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="M2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2496,15 +3008,15 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F6" s="8"/>
     </row>
@@ -2550,7 +3062,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B10" s="9"/>
     </row>

</xml_diff>

<commit_message>
validate and delete customer
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -14,14 +14,16 @@
     <sheet name="AssignUserToGroupModelerUI" sheetId="5" r:id="rId5"/>
     <sheet name="AddTagsToGroupTest" sheetId="6" r:id="rId6"/>
     <sheet name="AddProjectTest" sheetId="7" r:id="rId7"/>
-    <sheet name="AddTagTest" sheetId="8" r:id="rId8"/>
-    <sheet name="AddProjectTagAndDiagram" sheetId="9" r:id="rId9"/>
-    <sheet name="AddCustomer" sheetId="11" r:id="rId10"/>
-    <sheet name="ReuseDiagramAndObjects" sheetId="15" r:id="rId11"/>
-    <sheet name="AddDiagramWithObjectsAndLinks" sheetId="10" r:id="rId12"/>
-    <sheet name="DeleteUserModelerUI" sheetId="12" r:id="rId13"/>
-    <sheet name="DeleteGroupsModelerUI" sheetId="13" r:id="rId14"/>
-    <sheet name="DeleteCustomer" sheetId="14" r:id="rId15"/>
+    <sheet name="DeleteTagTest" sheetId="16" r:id="rId8"/>
+    <sheet name="AddTagTest" sheetId="8" r:id="rId9"/>
+    <sheet name="AddProjectTagAndDiagram" sheetId="9" r:id="rId10"/>
+    <sheet name="AddCustomer" sheetId="11" r:id="rId11"/>
+    <sheet name="ReuseDiagramAndObjects" sheetId="15" r:id="rId12"/>
+    <sheet name="AddDiagramWithObjectsAndLinks" sheetId="10" r:id="rId13"/>
+    <sheet name="DeleteUserModelerUI" sheetId="12" r:id="rId14"/>
+    <sheet name="DeleteGroupsModelerUI" sheetId="13" r:id="rId15"/>
+    <sheet name="DeleteCustomer" sheetId="14" r:id="rId16"/>
+    <sheet name="DeleteDiagram" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -661,7 +663,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -690,7 +692,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="135">
   <si>
     <t>Webelement</t>
   </si>
@@ -983,18 +985,9 @@
     <t>//div[normalize-space()='Test Delete Group']</t>
   </si>
   <si>
-    <t>Test Delete Account</t>
-  </si>
-  <si>
-    <t>delete.com</t>
-  </si>
-  <si>
     <t>verifyCustomer</t>
   </si>
   <si>
-    <t>//span[contains(text(),'Test Delete Account')]</t>
-  </si>
-  <si>
     <t>inputData1</t>
   </si>
   <si>
@@ -1055,12 +1048,6 @@
     <t>Knowledge Source-Nitesh (2)</t>
   </si>
   <si>
-    <t>Second Input name a</t>
-  </si>
-  <si>
-    <t>Knowledge name a</t>
-  </si>
-  <si>
     <t>Test Validation</t>
   </si>
   <si>
@@ -1070,19 +1057,46 @@
     <t>Test Validate Diagram</t>
   </si>
   <si>
-    <t>First Input name a</t>
-  </si>
-  <si>
-    <t>First decision a</t>
-  </si>
-  <si>
-    <t>Second decision a</t>
-  </si>
-  <si>
-    <t>Third decision a</t>
-  </si>
-  <si>
-    <t>Fourth decision a</t>
+    <t>Test dummy 9</t>
+  </si>
+  <si>
+    <t>Test Tag (94)</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Tag (94)')]</t>
+  </si>
+  <si>
+    <t>searchDiagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Test Create Diagram (14)</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Random')]</t>
+  </si>
+  <si>
+    <t>Knowledge name aa</t>
+  </si>
+  <si>
+    <t>First Input name ab</t>
+  </si>
+  <si>
+    <t>Second Input name ab</t>
+  </si>
+  <si>
+    <t>First decision ab</t>
+  </si>
+  <si>
+    <t>Second decision ab</t>
+  </si>
+  <si>
+    <t>Third decision ab</t>
+  </si>
+  <si>
+    <t>Fourth decision ab</t>
   </si>
 </sst>
 </file>
@@ -1676,10 +1690,244 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>-56</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>-30</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>70</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+      <c r="F8">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>155</v>
+      </c>
+      <c r="B11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>255</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>180</v>
+      </c>
+      <c r="B13">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-100</v>
+      </c>
+      <c r="B14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>180</v>
+      </c>
+      <c r="B15">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-250</v>
+      </c>
+      <c r="B16">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,13 +1958,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E2" t="s">
         <v>83</v>
@@ -1735,10 +1983,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1758,7 +2006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P22"/>
   <sheetViews>
@@ -1816,27 +2064,27 @@
         <v>56</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -1845,10 +2093,10 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -1860,28 +2108,28 @@
         <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J2" t="s">
         <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="L2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="N2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2078,12 +2326,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2145,7 +2393,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
         <v>41</v>
@@ -2154,10 +2402,10 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F2" t="s">
         <v>48</v>
@@ -2169,19 +2417,19 @@
         <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J2" t="s">
         <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="L2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="M2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2189,10 +2437,10 @@
         <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="M3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2200,12 +2448,12 @@
         <v>44</v>
       </c>
       <c r="M4" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2392,7 +2640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -2466,7 +2714,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2531,53 +2779,73 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" t="s">
-        <v>100</v>
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2889,6 +3157,62 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2934,238 +3258,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" t="s">
-        <v>115</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>-56</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>-30</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>250</v>
-      </c>
-      <c r="B8">
-        <v>70</v>
-      </c>
-      <c r="C8">
-        <v>150</v>
-      </c>
-      <c r="D8">
-        <v>70</v>
-      </c>
-      <c r="E8">
-        <v>300</v>
-      </c>
-      <c r="F8">
-        <v>-50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>155</v>
-      </c>
-      <c r="B11">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>255</v>
-      </c>
-      <c r="B12">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>180</v>
-      </c>
-      <c r="B13">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>-100</v>
-      </c>
-      <c r="B14">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>180</v>
-      </c>
-      <c r="B15">
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>-250</v>
-      </c>
-      <c r="B16">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A10:B10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
validate user and group
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="F2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,79 +89,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Project Administration xpath</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Folder Management xpath</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Banch Manager xpath</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Decision Modeler xpath</t>
+this xpath is used for deleting user, just change the email id before run then run the Delete User Script</t>
         </r>
       </text>
     </comment>
@@ -175,7 +103,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -195,11 +123,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Just change the name of the user to 'xyz' from the 'Test Undelete' place</t>
+Project Administration xpath</t>
         </r>
       </text>
     </comment>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -219,7 +147,55 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Just change the name of the group to 'xyz' from the 'Test Group' place</t>
+Folder Management xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Banch Manager xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision Modeler xpath</t>
         </r>
       </text>
     </comment>
@@ -233,7 +209,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -253,7 +229,31 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-These three are the xpath of branching, just copy and paste the xapth with the required branching in the first row and second column.</t>
+Just change the name of the user to 'xyz' from the 'Test Undelete' place</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Just change the name of the group to 'xyz' from the 'Test Group' place</t>
         </r>
       </text>
     </comment>
@@ -267,7 +267,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -287,118 +287,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Input data canvas coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Author:
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Decision data canvas coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-canvas value of knowledge coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-canvas value of goup coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-canvas value of annotation coordinates</t>
+These three are the xpath of branching, just copy and paste the xapth with the required branching in the first row and second column.</t>
         </r>
       </text>
     </comment>
@@ -557,7 +446,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="B14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -577,11 +466,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Project Administration xpath</t>
+Input data canvas coordinates</t>
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="A16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -591,21 +480,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Folder Management xpath</t>
+          <t xml:space="preserve">Author:
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -625,11 +505,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Banch Manager xpath</t>
+Decision data canvas coordinates</t>
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -649,7 +529,55 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Decision Modeler xpath</t>
+canvas value of knowledge coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of goup coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of annotation coordinates</t>
         </r>
       </text>
     </comment>
@@ -663,6 +591,112 @@
     <author>Author</author>
   </authors>
   <commentList>
+    <comment ref="C2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Project Administration xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Folder Management xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Banch Manager xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision Modeler xpath</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
     <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
@@ -692,7 +726,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="135">
   <si>
     <t>Webelement</t>
   </si>
@@ -733,15 +767,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>Test 6</t>
-  </si>
-  <si>
-    <t>Standard 6</t>
-  </si>
-  <si>
-    <t>test6@rxw.com</t>
-  </si>
-  <si>
     <t>STANDARD</t>
   </si>
   <si>
@@ -967,24 +992,12 @@
     <t>deleteuser@dummy.com</t>
   </si>
   <si>
-    <t>//div[normalize-space()='Test Delete User']</t>
-  </si>
-  <si>
     <t>deleteUser</t>
   </si>
   <si>
-    <t>Test Delete Group</t>
-  </si>
-  <si>
-    <t>test for delete group</t>
-  </si>
-  <si>
     <t>deleteGroup</t>
   </si>
   <si>
-    <t>//div[normalize-space()='Test Delete Group']</t>
-  </si>
-  <si>
     <t>verifyCustomer</t>
   </si>
   <si>
@@ -1097,6 +1110,27 @@
   </si>
   <si>
     <t>Fourth decision ab</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>defaultUserPass@123</t>
+  </si>
+  <si>
+    <t>Test Add</t>
+  </si>
+  <si>
+    <t>testadd@rxw.com</t>
+  </si>
+  <si>
+    <t>//div[normalize-space()='testadd@rxw.com']</t>
+  </si>
+  <si>
+    <t>User Delete</t>
+  </si>
+  <si>
+    <t>Test Group</t>
   </si>
 </sst>
 </file>
@@ -1637,10 +1671,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1651,10 +1685,10 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1712,107 +1746,107 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
       <c r="K2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" s="8"/>
     </row>
@@ -1858,7 +1892,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B10" s="9"/>
     </row>
@@ -1941,60 +1975,60 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" t="s">
         <v>83</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2034,133 +2068,133 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
       <c r="K2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="M2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="N2" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="O2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="P2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -2198,15 +2232,15 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E10" s="12"/>
       <c r="G10" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -2232,7 +2266,7 @@
     </row>
     <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B13" s="13"/>
     </row>
@@ -2330,7 +2364,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -2352,129 +2386,129 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" t="s">
+        <v>113</v>
+      </c>
+      <c r="J2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
-        <v>120</v>
-      </c>
-      <c r="J2" t="s">
-        <v>57</v>
-      </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="L2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="M2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="M3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -2512,15 +2546,15 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E10" s="12"/>
       <c r="G10" s="8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -2546,7 +2580,7 @@
     </row>
     <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B13" s="13"/>
     </row>
@@ -2645,7 +2679,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="E1" sqref="E1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,42 +2702,42 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2718,8 +2752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2732,30 +2766,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2795,18 +2829,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2830,17 +2864,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2850,70 +2884,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D5"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2922,7 +2972,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,21 +2984,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
@@ -2993,7 +3043,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>10</v>
@@ -3005,15 +3055,15 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3037,18 +3087,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -3074,27 +3124,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3119,34 +3169,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -3174,36 +3224,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3229,30 +3279,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added delete objects and validate
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -726,7 +726,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="134">
   <si>
     <t>Webelement</t>
   </si>
@@ -1082,36 +1082,9 @@
     <t>searchDiagram</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Test Create Diagram (14)</t>
-  </si>
-  <si>
     <t>//span[contains(text(),'Test Random')]</t>
   </si>
   <si>
-    <t>Knowledge name aa</t>
-  </si>
-  <si>
-    <t>First Input name ab</t>
-  </si>
-  <si>
-    <t>Second Input name ab</t>
-  </si>
-  <si>
-    <t>First decision ab</t>
-  </si>
-  <si>
-    <t>Second decision ab</t>
-  </si>
-  <si>
-    <t>Third decision ab</t>
-  </si>
-  <si>
-    <t>Fourth decision ab</t>
-  </si>
-  <si>
     <t>password</t>
   </si>
   <si>
@@ -1131,6 +1104,30 @@
   </si>
   <si>
     <t>Test Group</t>
+  </si>
+  <si>
+    <t>First Input name ad</t>
+  </si>
+  <si>
+    <t>Second Input name ad</t>
+  </si>
+  <si>
+    <t>Knowledge name ag</t>
+  </si>
+  <si>
+    <t>First decision ag</t>
+  </si>
+  <si>
+    <t>Second decision ag</t>
+  </si>
+  <si>
+    <t>Third decision ag</t>
+  </si>
+  <si>
+    <t>Fourth decision ag</t>
+  </si>
+  <si>
+    <t>Test Validate Diagram (9)</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2362,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2457,13 +2454,13 @@
         <v>54</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="L2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="M2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2471,10 +2468,10 @@
         <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2482,12 +2479,12 @@
         <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2722,7 +2719,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2752,7 +2749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -2780,7 +2777,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -2840,7 +2837,7 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2851,15 +2848,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -2868,13 +2865,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>118</v>
+      <c r="A2" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2915,7 +2907,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>88</v>
@@ -2923,22 +2915,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2995,7 +2987,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
added validation and report for tag
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="12" activeTab="16"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -63,6 +63,40 @@
 </comments>
 </file>
 
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Xpath for the customer needs to delete, just pass the customer name here itself</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -301,7 +335,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B14" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -309,7 +343,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -318,121 +352,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Input data canvas coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Author:
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Decision data canvas coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A20" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-canvas value of knowledge coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B21" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-canvas value of goup coordinates</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-canvas value of annotation coordinates</t>
+Just Change the name same as tag name before run the script</t>
         </r>
       </text>
     </comment>
@@ -591,7 +514,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="B14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -611,11 +534,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Project Administration xpath</t>
+Input data canvas coordinates</t>
         </r>
       </text>
     </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="A16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -625,21 +548,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Folder Management xpath</t>
+          <t xml:space="preserve">Author:
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -659,11 +573,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Banch Manager xpath</t>
+Decision data canvas coordinates</t>
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="A20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -683,7 +597,55 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Decision Modeler xpath</t>
+canvas value of knowledge coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of goup coordinates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+canvas value of annotation coordinates</t>
         </r>
       </text>
     </comment>
@@ -697,7 +659,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -705,7 +667,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -714,10 +676,82 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Xpath for the customer needs to delete, just pass the customer name here itself</t>
+Project Administration xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Folder Management xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Banch Manager xpath</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Decision Modeler xpath</t>
         </r>
       </text>
     </comment>
@@ -726,7 +760,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="134">
   <si>
     <t>Webelement</t>
   </si>
@@ -866,15 +900,9 @@
     <t>Test Tag</t>
   </si>
   <si>
-    <t>Dummy</t>
-  </si>
-  <si>
     <t>Twelve October</t>
   </si>
   <si>
-    <t>//span[normalize-space()='Test dummy 9 (main)']</t>
-  </si>
-  <si>
     <t>projectName1</t>
   </si>
   <si>
@@ -1070,15 +1098,6 @@
     <t>Test Validate Diagram</t>
   </si>
   <si>
-    <t>Test dummy 9</t>
-  </si>
-  <si>
-    <t>Test Tag (94)</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'Test Tag (94)')]</t>
-  </si>
-  <si>
     <t>searchDiagram</t>
   </si>
   <si>
@@ -1128,13 +1147,28 @@
   </si>
   <si>
     <t>Test Validate Diagram (9)</t>
+  </si>
+  <si>
+    <t>Test dummy8</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test dummy8 (main)']</t>
+  </si>
+  <si>
+    <t>Test Tag 8</t>
+  </si>
+  <si>
+    <t>Test Tag redo</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Tag redo')]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1197,6 +1231,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF474747"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1298,7 +1338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1341,6 +1381,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1755,7 +1796,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>43</v>
@@ -1764,27 +1805,27 @@
         <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -1793,34 +1834,34 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
         <v>58</v>
-      </c>
-      <c r="L2" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -1835,15 +1876,15 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F6" s="8"/>
     </row>
@@ -1889,7 +1930,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10" s="9"/>
     </row>
@@ -1972,60 +2013,60 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" t="s">
         <v>82</v>
-      </c>
-      <c r="F5" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2077,7 +2118,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>43</v>
@@ -2086,36 +2127,36 @@
         <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="J1" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -2124,43 +2165,43 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M2" t="s">
+        <v>96</v>
+      </c>
+      <c r="N2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" t="s">
         <v>107</v>
       </c>
-      <c r="J2" t="s">
-        <v>54</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>108</v>
-      </c>
-      <c r="M2" t="s">
-        <v>98</v>
-      </c>
-      <c r="N2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O2" t="s">
-        <v>109</v>
-      </c>
-      <c r="P2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2175,23 +2216,23 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -2229,15 +2270,15 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10" s="12"/>
       <c r="G10" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -2263,7 +2304,7 @@
     </row>
     <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="13"/>
     </row>
@@ -2395,7 +2436,7 @@
         <v>42</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>43</v>
@@ -2404,27 +2445,27 @@
         <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="M1" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -2433,34 +2474,34 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="L2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="M2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2468,10 +2509,10 @@
         <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="M3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2479,33 +2520,33 @@
         <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -2543,15 +2584,15 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B10" s="11"/>
       <c r="D10" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E10" s="12"/>
       <c r="G10" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H10" s="8"/>
     </row>
@@ -2577,7 +2618,7 @@
     </row>
     <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B13" s="13"/>
     </row>
@@ -2702,24 +2743,24 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2772,12 +2813,12 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -2826,18 +2867,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2850,7 +2891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
@@ -2861,12 +2902,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2907,30 +2948,30 @@
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2987,7 +3028,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -3172,7 +3213,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -3198,58 +3239,39 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>114</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3258,14 +3280,14 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3285,16 +3307,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add decision and input properties
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -1345,6 +1345,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1381,7 +1382,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1875,18 +1875,18 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1929,10 +1929,10 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="9"/>
+      <c r="B10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2215,26 +2215,26 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="10" t="s">
+      <c r="H7" s="18"/>
+      <c r="I7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2269,18 +2269,18 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="D10" s="12" t="s">
+      <c r="B10" s="12"/>
+      <c r="D10" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="G10" s="8" t="s">
+      <c r="E10" s="13"/>
+      <c r="G10" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2303,10 +2303,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2529,26 +2529,26 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="16" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="17"/>
-      <c r="I7" s="10" t="s">
+      <c r="H7" s="18"/>
+      <c r="I7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2583,18 +2583,18 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="D10" s="12" t="s">
+      <c r="B10" s="12"/>
+      <c r="D10" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="G10" s="8" t="s">
+      <c r="E10" s="13"/>
+      <c r="G10" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2617,10 +2617,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="13"/>
+      <c r="B13" s="14"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -3144,8 +3144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,7 +3242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
@@ -3261,7 +3261,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="6" t="s">
         <v>132</v>
       </c>
       <c r="B2" t="s">

</xml_diff>

<commit_message>
change password and implementation with knowledge properties
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="12" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="DeleteGroupsModelerUI" sheetId="13" r:id="rId15"/>
     <sheet name="DeleteCustomer" sheetId="14" r:id="rId16"/>
     <sheet name="DeleteDiagram" sheetId="17" r:id="rId17"/>
+    <sheet name="ChangePassword" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -97,6 +98,40 @@
 </comments>
 </file>
 
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Before running the script just update the password with the new one then run the script</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -760,7 +795,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="139">
   <si>
     <t>Webelement</t>
   </si>
@@ -1162,6 +1197,21 @@
   </si>
   <si>
     <t>//span[contains(text(),'Test Tag redo')]</t>
+  </si>
+  <si>
+    <t>changepassword@rxw.com</t>
+  </si>
+  <si>
+    <t>Welcome@123</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>userPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1382,6 +1432,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2916,6 +2967,53 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
@@ -3144,7 +3242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added change password, implementation data & delete object properties
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="12" activeTab="17"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="DeleteCustomer" sheetId="14" r:id="rId16"/>
     <sheet name="DeleteDiagram" sheetId="17" r:id="rId17"/>
     <sheet name="ChangePassword" sheetId="18" r:id="rId18"/>
+    <sheet name="DeleteObjectProperties" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -795,7 +796,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="141">
   <si>
     <t>Webelement</t>
   </si>
@@ -1212,6 +1213,12 @@
   </si>
   <si>
     <t>newPassword</t>
+  </si>
+  <si>
+    <t>searchObjectProperties</t>
+  </si>
+  <si>
+    <t>Implementation Data Updated</t>
   </si>
 </sst>
 </file>
@@ -1396,6 +1403,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1432,7 +1440,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1926,18 +1933,18 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1980,10 +1987,10 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="10"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2266,26 +2273,26 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="18"/>
+      <c r="G7" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="11" t="s">
+      <c r="H7" s="19"/>
+      <c r="I7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2320,18 +2327,18 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="13"/>
+      <c r="D10" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="G10" s="9" t="s">
+      <c r="E10" s="14"/>
+      <c r="G10" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2354,10 +2361,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="14"/>
+      <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2580,26 +2587,26 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="18"/>
+      <c r="G7" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="H7" s="18"/>
-      <c r="I7" s="11" t="s">
+      <c r="H7" s="19"/>
+      <c r="I7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="11"/>
+      <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -2634,18 +2641,18 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="D10" s="13" t="s">
+      <c r="B10" s="13"/>
+      <c r="D10" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="G10" s="9" t="s">
+      <c r="E10" s="14"/>
+      <c r="G10" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="9"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2668,10 +2675,10 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="14"/>
+      <c r="B13" s="15"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -2971,7 +2978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
@@ -2992,7 +2999,7 @@
       <c r="C1" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="19"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3011,6 +3018,34 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add project & tag multi user
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
     <sheet name="DeleteObjectProperties" sheetId="19" r:id="rId19"/>
     <sheet name="MultiUser" sheetId="20" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -763,7 +763,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="154">
   <si>
     <t>Webelement</t>
   </si>
@@ -990,9 +990,6 @@
     <t>domains</t>
   </si>
   <si>
-    <t>Test dummy</t>
-  </si>
-  <si>
     <t>User 1</t>
   </si>
   <si>
@@ -1222,6 +1219,12 @@
   </si>
   <si>
     <t>Re-used Objects Coordinates</t>
+  </si>
+  <si>
+    <t>multiuser test</t>
+  </si>
+  <si>
+    <t>Test MultiUser 6</t>
   </si>
 </sst>
 </file>
@@ -1889,7 +1892,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -1898,10 +1901,10 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
         <v>102</v>
-      </c>
-      <c r="E2" t="s">
-        <v>103</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -1913,7 +1916,7 @@
         <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J2" t="s">
         <v>52</v>
@@ -2086,51 +2089,51 @@
         <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2200,27 +2203,27 @@
         <v>51</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -2229,10 +2232,10 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
         <v>102</v>
-      </c>
-      <c r="E2" t="s">
-        <v>103</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -2244,28 +2247,28 @@
         <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J2" t="s">
         <v>52</v>
       </c>
       <c r="K2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
         <v>95</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
+        <v>96</v>
+      </c>
+      <c r="O2" t="s">
         <v>106</v>
       </c>
-      <c r="M2" t="s">
-        <v>96</v>
-      </c>
-      <c r="N2" t="s">
-        <v>97</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>107</v>
-      </c>
-      <c r="P2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -2529,7 +2532,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -2538,10 +2541,10 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" t="s">
-        <v>110</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -2553,19 +2556,19 @@
         <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J2" t="s">
         <v>52</v>
       </c>
       <c r="K2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" t="s">
+        <v>120</v>
+      </c>
+      <c r="M2" t="s">
         <v>123</v>
-      </c>
-      <c r="L2" t="s">
-        <v>121</v>
-      </c>
-      <c r="M2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2573,10 +2576,10 @@
         <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2584,12 +2587,12 @@
         <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -2807,24 +2810,24 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
         <v>83</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2877,12 +2880,12 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -2934,15 +2937,15 @@
         <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2966,12 +2969,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -2997,25 +3000,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="B2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3041,12 +3044,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3086,30 +3089,30 @@
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3140,10 +3143,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3164,27 +3167,27 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L1" s="20"/>
     </row>
@@ -3266,65 +3269,103 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>-35</v>
+      </c>
+      <c r="B8">
+        <v>-65</v>
+      </c>
+      <c r="C8">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>-45</v>
+      </c>
+      <c r="G8">
+        <v>70</v>
+      </c>
+      <c r="H8">
+        <v>-65</v>
+      </c>
+      <c r="I8">
+        <v>85</v>
+      </c>
+      <c r="J8">
+        <v>55</v>
+      </c>
+      <c r="K8">
+        <v>-35</v>
+      </c>
+      <c r="L8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>-95</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>-195</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>105</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>105</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>55</v>
       </c>
-      <c r="F8">
+      <c r="F10">
         <v>-135</v>
       </c>
-      <c r="G8">
+      <c r="G10">
         <v>205</v>
       </c>
-      <c r="H8">
+      <c r="H10">
         <v>-195</v>
       </c>
-      <c r="I8">
+      <c r="I10">
         <v>255</v>
       </c>
-      <c r="J8">
+      <c r="J10">
         <v>155</v>
       </c>
-      <c r="K8">
+      <c r="K10">
         <v>-95</v>
       </c>
-      <c r="L8">
+      <c r="L10">
         <v>85</v>
       </c>
     </row>
@@ -3376,7 +3417,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -3537,14 +3578,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3561,10 +3602,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
@@ -3610,10 +3651,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" t="s">
         <v>132</v>
-      </c>
-      <c r="B2" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -3655,13 +3696,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" t="s">
         <v>129</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>130</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
validation of project and tag for multiuser
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -328,6 +328,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+For validation in MultiUser, keep "projectName" &amp; "xpathVerifyProject" name same</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -763,7 +787,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="158">
   <si>
     <t>Webelement</t>
   </si>
@@ -1149,12 +1173,6 @@
     <t>Test Validate Diagram (9)</t>
   </si>
   <si>
-    <t>Test dummy8</t>
-  </si>
-  <si>
-    <t>//span[normalize-space()='Test dummy8 (main)']</t>
-  </si>
-  <si>
     <t>Test Tag 8</t>
   </si>
   <si>
@@ -1224,7 +1242,25 @@
     <t>multiuser test</t>
   </si>
   <si>
-    <t>Test MultiUser 6</t>
+    <t>xpathverifyTag</t>
+  </si>
+  <si>
+    <t>xpathverifyProject</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test MultiUser 17')]</t>
+  </si>
+  <si>
+    <t>Test MultiUser 17</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test MultiUser 17 (main)']</t>
+  </si>
+  <si>
+    <t>Test MultiUser 18</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test MultiUser 18')]</t>
   </si>
 </sst>
 </file>
@@ -2923,7 +2959,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3000,25 +3036,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
         <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -3044,12 +3080,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3167,27 +3203,27 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L1" s="20"/>
     </row>
@@ -3269,27 +3305,27 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H7" s="20"/>
       <c r="I7" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L7" s="20"/>
     </row>
@@ -3576,20 +3612,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -3599,24 +3636,30 @@
       <c r="C1" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>41</v>
       </c>
@@ -3651,10 +3694,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3666,21 +3709,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>42</v>
       </c>
@@ -3693,19 +3737,25 @@
       <c r="D1" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" t="s">
         <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" t="s">
-        <v>130</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
crud operation of tag
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -787,7 +787,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="164">
   <si>
     <t>Webelement</t>
   </si>
@@ -1261,6 +1261,24 @@
   </si>
   <si>
     <t>//span[contains(text(),'Test MultiUser 18')]</t>
+  </si>
+  <si>
+    <t>xpathUpdateTag</t>
+  </si>
+  <si>
+    <t>updateName</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Tag 8')]</t>
+  </si>
+  <si>
+    <t>Test Tag 8 Update</t>
+  </si>
+  <si>
+    <t>xpathVerifyTag</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Tag 8 Update')]</t>
   </si>
 </sst>
 </file>
@@ -3489,7 +3507,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3614,7 +3632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
@@ -3709,18 +3727,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3758,6 +3776,28 @@
         <v>153</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
multiple user with diagram
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="13" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -3199,8 +3199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3321,69 +3321,55 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-130</v>
+      </c>
+      <c r="B4">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-10</v>
+      </c>
+      <c r="B6">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20" t="s">
+      <c r="D9" s="20"/>
+      <c r="E9" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20" t="s">
+      <c r="F9" s="20"/>
+      <c r="G9" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20" t="s">
+      <c r="H9" s="20"/>
+      <c r="I9" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20" t="s">
+      <c r="J9" s="20"/>
+      <c r="K9" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="L7" s="20"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>-35</v>
-      </c>
-      <c r="B8">
-        <v>-65</v>
-      </c>
-      <c r="C8">
-        <v>35</v>
-      </c>
-      <c r="D8">
-        <v>35</v>
-      </c>
-      <c r="E8">
-        <v>20</v>
-      </c>
-      <c r="F8">
-        <v>-45</v>
-      </c>
-      <c r="G8">
-        <v>70</v>
-      </c>
-      <c r="H8">
-        <v>-65</v>
-      </c>
-      <c r="I8">
-        <v>85</v>
-      </c>
-      <c r="J8">
-        <v>55</v>
-      </c>
-      <c r="K8">
-        <v>-35</v>
-      </c>
-      <c r="L8">
-        <v>30</v>
-      </c>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -3426,12 +3412,12 @@
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
@@ -3729,7 +3715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
create & delete branch, export & import project
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="14" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="ChangePassword" sheetId="18" r:id="rId18"/>
     <sheet name="DeleteObjectProperties" sheetId="19" r:id="rId19"/>
     <sheet name="MultiUser" sheetId="20" r:id="rId20"/>
+    <sheet name="Branch" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -787,7 +788,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
   <si>
     <t>Webelement</t>
   </si>
@@ -1113,12 +1114,6 @@
     <t>Knowledge Source-Nitesh (2)</t>
   </si>
   <si>
-    <t>Test Validation</t>
-  </si>
-  <si>
-    <t>//span[normalize-space()='Test Validation (main)']</t>
-  </si>
-  <si>
     <t>Test Validate Diagram</t>
   </si>
   <si>
@@ -1279,6 +1274,63 @@
   </si>
   <si>
     <t>//span[contains(text(),'Test Tag 8 Update')]</t>
+  </si>
+  <si>
+    <t>Test Run</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test Run (main)']</t>
+  </si>
+  <si>
+    <t>ExportType</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Standard DMN']</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Camunda DMN']</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Red Hat DMN']</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='IBM ADS Zip']</t>
+  </si>
+  <si>
+    <t>Test Automation (1)</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='main']</t>
+  </si>
+  <si>
+    <t>branchName</t>
+  </si>
+  <si>
+    <t>Testing Branch</t>
+  </si>
+  <si>
+    <t>creating branch under tag</t>
+  </si>
+  <si>
+    <t>branchXpath</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Testing Branch')]</t>
+  </si>
+  <si>
+    <t>Import Tag (9)</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Import Tag (9)']</t>
+  </si>
+  <si>
+    <t>searchBranch</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='gg (1)']</t>
+  </si>
+  <si>
+    <t>gg (1)</t>
   </si>
 </sst>
 </file>
@@ -2521,10 +2573,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,16 +2586,18 @@
     <col min="3" max="3" width="68.28515625" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -2583,10 +2637,13 @@
       <c r="M1" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -2595,10 +2652,10 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -2610,46 +2667,64 @@
         <v>49</v>
       </c>
       <c r="I2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J2" t="s">
         <v>52</v>
       </c>
       <c r="K2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="N2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>40</v>
       </c>
+      <c r="F3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H3" t="s">
+        <v>177</v>
+      </c>
       <c r="L3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="N3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>41</v>
       </c>
       <c r="M4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="N4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="N5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>63</v>
       </c>
@@ -2671,7 +2746,7 @@
       </c>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-30</v>
       </c>
@@ -2703,7 +2778,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>68</v>
       </c>
@@ -2717,7 +2792,7 @@
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-43</v>
       </c>
@@ -2737,13 +2812,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="15"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2751,7 +2826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-100</v>
       </c>
@@ -2759,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>250</v>
       </c>
@@ -2881,7 +2956,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2939,7 +3014,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -2999,7 +3074,7 @@
         <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -3023,12 +3098,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3054,25 +3129,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>135</v>
       </c>
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3098,12 +3173,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -3143,7 +3218,7 @@
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>85</v>
@@ -3151,22 +3226,22 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3199,7 +3274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
@@ -3221,27 +3296,27 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="L1" s="20"/>
     </row>
@@ -3347,27 +3422,27 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="L9" s="20"/>
     </row>
@@ -3426,6 +3501,84 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3457,7 +3610,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
@@ -3641,21 +3794,21 @@
         <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,10 +3851,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3716,13 +3869,13 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
@@ -3742,46 +3895,46 @@
         <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" t="s">
         <v>161</v>
-      </c>
-      <c r="C6" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integration of customer adding to create diagram
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="14" activeTab="20"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="AddGroupsModelerUIWithDifferent" sheetId="1" r:id="rId1"/>
@@ -788,7 +788,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="179">
   <si>
     <t>Webelement</t>
   </si>
@@ -1165,18 +1165,6 @@
     <t>Fourth decision ag</t>
   </si>
   <si>
-    <t>Test Validate Diagram (9)</t>
-  </si>
-  <si>
-    <t>Test Tag 8</t>
-  </si>
-  <si>
-    <t>Test Tag redo</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'Test Tag redo')]</t>
-  </si>
-  <si>
     <t>changepassword@rxw.com</t>
   </si>
   <si>
@@ -1234,30 +1222,12 @@
     <t>Re-used Objects Coordinates</t>
   </si>
   <si>
-    <t>multiuser test</t>
-  </si>
-  <si>
     <t>xpathverifyTag</t>
   </si>
   <si>
     <t>xpathverifyProject</t>
   </si>
   <si>
-    <t>//span[contains(text(),'Test MultiUser 17')]</t>
-  </si>
-  <si>
-    <t>Test MultiUser 17</t>
-  </si>
-  <si>
-    <t>//span[normalize-space()='Test MultiUser 17 (main)']</t>
-  </si>
-  <si>
-    <t>Test MultiUser 18</t>
-  </si>
-  <si>
-    <t>//span[contains(text(),'Test MultiUser 18')]</t>
-  </si>
-  <si>
     <t>xpathUpdateTag</t>
   </si>
   <si>
@@ -1331,6 +1301,30 @@
   </si>
   <si>
     <t>gg (1)</t>
+  </si>
+  <si>
+    <t>sample demo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Tag </t>
+  </si>
+  <si>
+    <t>Sixteenth Feburary</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Tag')]</t>
+  </si>
+  <si>
+    <t>Test Sample</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Sample')]</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test Sample (main)']</t>
+  </si>
+  <si>
+    <t>Test Diagram</t>
   </si>
 </sst>
 </file>
@@ -1937,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,13 +1940,16 @@
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -2575,8 +2572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2638,12 +2635,12 @@
         <v>54</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
         <v>38</v>
@@ -2652,10 +2649,10 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
         <v>45</v>
@@ -2682,7 +2679,7 @@
         <v>121</v>
       </c>
       <c r="N2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2690,10 +2687,10 @@
         <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="H3" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="L3" t="s">
         <v>119</v>
@@ -2702,7 +2699,7 @@
         <v>122</v>
       </c>
       <c r="N3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2713,7 +2710,7 @@
         <v>123</v>
       </c>
       <c r="N4" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2721,7 +2718,7 @@
         <v>124</v>
       </c>
       <c r="N5" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -3088,7 +3085,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,7 +3100,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -3129,25 +3126,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -3173,12 +3170,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3191,7 +3188,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3296,27 +3293,27 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D1" s="20"/>
       <c r="E1" s="20" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="20" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J1" s="20"/>
       <c r="K1" s="20" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="L1" s="20"/>
     </row>
@@ -3422,27 +3419,27 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D9" s="20"/>
       <c r="E9" s="20" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="20" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="L9" s="20"/>
     </row>
@@ -3508,7 +3505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
@@ -3529,38 +3526,38 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D2" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -3568,13 +3565,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B6" t="s">
         <v>169</v>
       </c>
-      <c r="B6" t="s">
-        <v>179</v>
-      </c>
       <c r="C6" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3587,7 +3584,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3769,10 +3766,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3781,9 +3778,16 @@
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>36</v>
       </c>
@@ -3793,37 +3797,194 @@
       <c r="C1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>41</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>-56</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>-30</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>250</v>
+      </c>
+      <c r="B8">
+        <v>70</v>
+      </c>
+      <c r="C8">
+        <v>150</v>
+      </c>
+      <c r="D8">
+        <v>70</v>
+      </c>
+      <c r="E8">
+        <v>300</v>
+      </c>
+      <c r="F8">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>155</v>
+      </c>
+      <c r="B11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>255</v>
+      </c>
+      <c r="B12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>180</v>
+      </c>
+      <c r="B13">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-100</v>
+      </c>
+      <c r="B14">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>180</v>
+      </c>
+      <c r="B15">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>-250</v>
+      </c>
+      <c r="B16">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3832,12 +3993,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3851,10 +4012,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3869,7 +4030,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3877,7 +4038,7 @@
     <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3895,46 +4056,46 @@
         <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>172</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B6" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set branch as Active
</commit_message>
<xml_diff>
--- a/Test Data/TestData.xlsx
+++ b/Test Data/TestData.xlsx
@@ -353,6 +353,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="G3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+it's used to delete the diagram of "DeleteDiagramAndObjectsUsingSearch" class</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -788,7 +812,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="179">
   <si>
     <t>Webelement</t>
   </si>
@@ -1267,9 +1291,6 @@
     <t>//span[normalize-space()='IBM ADS Zip']</t>
   </si>
   <si>
-    <t>Test Automation (1)</t>
-  </si>
-  <si>
     <t>//span[normalize-space()='main']</t>
   </si>
   <si>
@@ -1297,12 +1318,6 @@
     <t>searchBranch</t>
   </si>
   <si>
-    <t>//span[normalize-space()='gg (1)']</t>
-  </si>
-  <si>
-    <t>gg (1)</t>
-  </si>
-  <si>
     <t>sample demo</t>
   </si>
   <si>
@@ -1321,10 +1336,19 @@
     <t>//span[contains(text(),'Test Sample')]</t>
   </si>
   <si>
-    <t>//span[normalize-space()='Test Sample (main)']</t>
-  </si>
-  <si>
     <t>Test Diagram</t>
+  </si>
+  <si>
+    <t>Diagram</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Testing Branch']</t>
+  </si>
+  <si>
+    <t>//span[normalize-space()='Test Sample (Testing Branch)']</t>
+  </si>
+  <si>
+    <t>//span[contains(text(),'Test Sample (Testing Branch)')]</t>
   </si>
 </sst>
 </file>
@@ -2687,10 +2711,10 @@
         <v>40</v>
       </c>
       <c r="F3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" t="s">
         <v>166</v>
-      </c>
-      <c r="H3" t="s">
-        <v>167</v>
       </c>
       <c r="L3" t="s">
         <v>119</v>
@@ -3085,7 +3109,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,7 +3124,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -3506,7 +3530,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3526,38 +3550,38 @@
         <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
         <v>159</v>
       </c>
-      <c r="B2" t="s">
-        <v>160</v>
-      </c>
       <c r="C2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" t="s">
         <v>162</v>
       </c>
-      <c r="D2" t="s">
-        <v>163</v>
-      </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>42</v>
@@ -3565,13 +3589,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3769,7 +3793,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3824,25 +3848,25 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s">
         <v>49</v>
       </c>
       <c r="G2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H2" t="s">
         <v>52</v>
@@ -3860,6 +3884,9 @@
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -4015,7 +4042,7 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -4030,16 +4057,16 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4061,19 +4088,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B2" t="s">
         <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>